<commit_message>
updates to quiz template
</commit_message>
<xml_diff>
--- a/inst/templates/quiz_template.xlsx
+++ b/inst/templates/quiz_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\andreashandel\quizgrader\inst\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\andreashandel\quizgrader\inst\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F3C9A-E080-4980-B3F6-CBC4B7DEEC26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA91066D-D202-4AA6-A970-C76C33969FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4170" yWindow="1830" windowWidth="51300" windowHeight="20595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Answer</t>
   </si>
@@ -137,9 +137,6 @@
     <t>remember that [] means the numbers at the ends of the ranges are also included</t>
   </si>
   <si>
-    <t>this would allow wrong rounding of the answer to e.g. 41</t>
-  </si>
-  <si>
     <t>quiz1</t>
   </si>
   <si>
@@ -177,13 +174,69 @@
   </si>
   <si>
     <t>DueDate</t>
+  </si>
+  <si>
+    <t>A single character is expected and only the first character is evaluated. Capitalization is ignored.</t>
+  </si>
+  <si>
+    <t>Leading and trailing white spaces are trimmed in the submission and capitalization is ignored, but otherwise matching is strict.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Expected inputs are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>True/False, Yes/No,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>1/0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Only the first character is evaluated (i.e.  T/Y/1 or F/N/0). Capitalization is ignored. Any non-match is considered a mistake.</t>
+    </r>
+  </si>
+  <si>
+    <t>Expect an integer number. Anything non-integer or non-matching is considered incorrect.</t>
+  </si>
+  <si>
+    <t>This  allows wrong rounding of the answer to e.g. 41</t>
+  </si>
+  <si>
+    <t>A numeric value rounded to some specified significant digits. Those digits need to match the provided answer.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +263,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -591,9 +649,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -606,9 +666,9 @@
     <col min="9" max="10" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
@@ -632,18 +692,18 @@
         <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>29</v>
@@ -660,6 +720,9 @@
       <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
       <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
@@ -667,12 +730,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>20</v>
@@ -687,6 +750,9 @@
       <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
@@ -694,12 +760,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="90">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -714,6 +780,9 @@
       <c r="G4" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
       <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
@@ -721,12 +790,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>19</v>
@@ -743,6 +812,9 @@
       <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
       <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
@@ -750,12 +822,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>33</v>
@@ -767,13 +839,13 @@
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>10</v>
@@ -782,12 +854,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>32</v>
@@ -802,7 +874,7 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>10</v>
@@ -811,12 +883,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>31</v>
@@ -828,10 +900,13 @@
         <v>42.42</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>10</v>
@@ -843,5 +918,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>